<commit_message>
cenarios de cadastro de buscalupa criados.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-appium-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-appium-bdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FAFC6F-7FE3-4D38-8BBA-02A0A1FE7A7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8B3F5E-D0AC-437D-8775-BC0A452E5BF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
@@ -213,7 +213,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>lucascarvalh26</t>
+    <t>lucascarvalh28</t>
   </si>
 </sst>
 </file>

</xml_diff>